<commit_message>
Fix  Run command bug
</commit_message>
<xml_diff>
--- a/Data/Input/Uipath界面.xlsx
+++ b/Data/Input/Uipath界面.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hank H Liu\Documents\UiPath\Uipath\Data\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophie J He\Documents\Uipath\GSS-\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40739F78-3DD3-4ECA-8F6B-CEF294761344}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BDF22E8-C597-47F3-BBB7-454C543A5571}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{2B77C280-2D13-4499-900C-E0EEFD2412A6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{2B77C280-2D13-4499-900C-E0EEFD2412A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -571,7 +571,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -620,7 +620,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -651,13 +651,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -706,7 +706,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -737,13 +737,13 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -792,7 +792,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -829,7 +829,7 @@
           <xdr:col>5</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -878,7 +878,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -915,7 +915,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -964,7 +964,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1001,7 +1001,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1050,7 +1050,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1081,13 +1081,13 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1136,7 +1136,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1167,13 +1167,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1222,7 +1222,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1253,13 +1253,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>24</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1308,7 +1308,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1345,7 +1345,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1394,7 +1394,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1431,7 +1431,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1480,7 +1480,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1517,7 +1517,7 @@
           <xdr:col>3</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>27</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1566,7 +1566,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1597,13 +1597,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1652,7 +1652,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1681,9 +1681,9 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>66675</xdr:colOff>
+          <xdr:colOff>68580</xdr:colOff>
           <xdr:row>36</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
@@ -1738,7 +1738,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1767,15 +1767,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>5</xdr:col>
-          <xdr:colOff>66675</xdr:colOff>
+          <xdr:colOff>68580</xdr:colOff>
           <xdr:row>1</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>114300</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1824,7 +1824,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1853,15 +1853,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
+          <xdr:colOff>60960</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>790575</xdr:colOff>
+          <xdr:colOff>792480</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1910,7 +1910,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -1939,15 +1939,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>133350</xdr:colOff>
+          <xdr:colOff>137160</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>22860</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1996,7 +1996,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2025,15 +2025,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>133350</xdr:colOff>
+          <xdr:colOff>137160</xdr:colOff>
           <xdr:row>32</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>22860</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2082,7 +2082,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2113,13 +2113,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>42</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>333375</xdr:colOff>
+          <xdr:colOff>335280</xdr:colOff>
           <xdr:row>44</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2168,7 +2168,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2197,15 +2197,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>95250</xdr:colOff>
+          <xdr:colOff>99060</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>22860</xdr:colOff>
           <xdr:row>30</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2254,7 +2254,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2285,13 +2285,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2340,7 +2340,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2369,15 +2369,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>133350</xdr:colOff>
+          <xdr:colOff>137160</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>57150</xdr:colOff>
+          <xdr:colOff>60960</xdr:colOff>
           <xdr:row>15</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2426,7 +2426,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2466,9 +2466,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2517,7 +2517,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2552,9 +2552,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2603,7 +2603,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2634,13 +2634,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>3</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2689,7 +2689,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2724,9 +2724,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2775,7 +2775,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2810,9 +2810,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>11</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2861,7 +2861,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2896,9 +2896,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>34</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2947,7 +2947,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -2978,13 +2978,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>10</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3033,7 +3033,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3064,13 +3064,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>16</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>18</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3119,7 +3119,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3150,13 +3150,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>29</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>31</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3205,7 +3205,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3236,13 +3236,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>33</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>35</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3291,7 +3291,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3326,9 +3326,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>25</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3377,7 +3377,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3412,9 +3412,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>19</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3463,7 +3463,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3498,9 +3498,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>38</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3549,7 +3549,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3578,13 +3578,13 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>133350</xdr:colOff>
+          <xdr:colOff>137160</xdr:colOff>
           <xdr:row>44</xdr:row>
-          <xdr:rowOff>133350</xdr:rowOff>
+          <xdr:rowOff>137160</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>866775</xdr:colOff>
+          <xdr:colOff>868680</xdr:colOff>
           <xdr:row>46</xdr:row>
           <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
@@ -3635,7 +3635,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3664,15 +3664,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>161925</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>895350</xdr:colOff>
+          <xdr:colOff>899160</xdr:colOff>
           <xdr:row>7</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3721,7 +3721,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3750,15 +3750,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>161925</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>895350</xdr:colOff>
+          <xdr:colOff>899160</xdr:colOff>
           <xdr:row>13</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3807,7 +3807,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3842,9 +3842,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>1619250</xdr:colOff>
+          <xdr:colOff>1623060</xdr:colOff>
           <xdr:row>42</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3893,7 +3893,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -3928,9 +3928,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>1619250</xdr:colOff>
+          <xdr:colOff>1623060</xdr:colOff>
           <xdr:row>43</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3979,7 +3979,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4008,15 +4008,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>85725</xdr:colOff>
+          <xdr:colOff>83820</xdr:colOff>
           <xdr:row>47</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>819150</xdr:colOff>
+          <xdr:colOff>822960</xdr:colOff>
           <xdr:row>49</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4065,7 +4065,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4096,13 +4096,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>37</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
+          <xdr:rowOff>160020</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>39</xdr:row>
-          <xdr:rowOff>66675</xdr:rowOff>
+          <xdr:rowOff>68580</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4151,7 +4151,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4182,13 +4182,13 @@
           <xdr:col>1</xdr:col>
           <xdr:colOff>152400</xdr:colOff>
           <xdr:row>26</xdr:row>
-          <xdr:rowOff>142875</xdr:rowOff>
+          <xdr:rowOff>144780</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>885825</xdr:colOff>
+          <xdr:colOff>883920</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>45720</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4237,7 +4237,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4266,15 +4266,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>161925</xdr:colOff>
+          <xdr:colOff>160020</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>895350</xdr:colOff>
+          <xdr:colOff>899160</xdr:colOff>
           <xdr:row>22</xdr:row>
-          <xdr:rowOff>57150</xdr:rowOff>
+          <xdr:rowOff>60960</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4323,7 +4323,7 @@
             </a:extLst>
           </xdr:spPr>
           <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
+            <a:bodyPr vertOverflow="clip" wrap="square" lIns="36576" tIns="32004" rIns="0" bIns="32004" anchor="ctr" upright="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr algn="l" rtl="0">
@@ -4654,10 +4654,10 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.140625" style="3" customWidth="1"/>
-    <col min="2" max="5" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" style="3" customWidth="1"/>
+    <col min="2" max="5" width="10.6640625" customWidth="1"/>
     <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4896,7 +4896,7 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4912,13 +4912,13 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>0</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4934,13 +4934,13 @@
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>4</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4962,7 +4962,7 @@
                     <xdr:col>5</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4984,7 +4984,7 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5006,7 +5006,7 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5022,13 +5022,13 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>45720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5044,13 +5044,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5066,13 +5066,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>24</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5094,7 +5094,7 @@
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>18</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5116,7 +5116,7 @@
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5138,7 +5138,7 @@
                     <xdr:col>3</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>27</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5154,13 +5154,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>30</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>45720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5174,9 +5174,9 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:colOff>68580</xdr:colOff>
                     <xdr:row>36</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
@@ -5196,15 +5196,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>5</xdr:col>
-                    <xdr:colOff>66675</xdr:colOff>
+                    <xdr:colOff>68580</xdr:colOff>
                     <xdr:row>1</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>7</xdr:col>
                     <xdr:colOff>114300</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>45720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5218,15 +5218,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:colOff>60960</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>790575</xdr:colOff>
+                    <xdr:colOff>792480</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5240,15 +5240,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>133350</xdr:colOff>
+                    <xdr:colOff>137160</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>22860</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5262,15 +5262,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>133350</xdr:colOff>
+                    <xdr:colOff>137160</xdr:colOff>
                     <xdr:row>32</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>22860</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5286,13 +5286,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>42</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>333375</xdr:colOff>
+                    <xdr:colOff>335280</xdr:colOff>
                     <xdr:row>44</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>45720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5306,15 +5306,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>95250</xdr:colOff>
+                    <xdr:colOff>99060</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>3</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
+                    <xdr:colOff>22860</xdr:colOff>
                     <xdr:row>30</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>45720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5330,13 +5330,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>21</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>45720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5350,15 +5350,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>133350</xdr:colOff>
+                    <xdr:colOff>137160</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>2</xdr:col>
-                    <xdr:colOff>57150</xdr:colOff>
+                    <xdr:colOff>60960</xdr:colOff>
                     <xdr:row>15</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>45720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5376,16 +5376,16 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="88" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="112.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="112.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -5653,9 +5653,9 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5675,9 +5675,9 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5693,13 +5693,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>3</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5719,9 +5719,9 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>6</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5741,9 +5741,9 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>11</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5763,9 +5763,9 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>34</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5781,13 +5781,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>10</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>12</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5803,13 +5803,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>16</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>18</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5825,13 +5825,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>29</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>31</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5847,13 +5847,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>33</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>35</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5873,9 +5873,9 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>25</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5895,9 +5895,9 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>19</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5917,9 +5917,9 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>38</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5933,13 +5933,13 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>133350</xdr:colOff>
+                    <xdr:colOff>137160</xdr:colOff>
                     <xdr:row>44</xdr:row>
-                    <xdr:rowOff>133350</xdr:rowOff>
+                    <xdr:rowOff>137160</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>866775</xdr:colOff>
+                    <xdr:colOff>868680</xdr:colOff>
                     <xdr:row>46</xdr:row>
                     <xdr:rowOff>38100</xdr:rowOff>
                   </to>
@@ -5955,15 +5955,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>161925</xdr:colOff>
+                    <xdr:colOff>160020</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>895350</xdr:colOff>
+                    <xdr:colOff>899160</xdr:colOff>
                     <xdr:row>7</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>45720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5977,15 +5977,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>161925</xdr:colOff>
+                    <xdr:colOff>160020</xdr:colOff>
                     <xdr:row>11</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>895350</xdr:colOff>
+                    <xdr:colOff>899160</xdr:colOff>
                     <xdr:row>13</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6005,9 +6005,9 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>1619250</xdr:colOff>
+                    <xdr:colOff>1623060</xdr:colOff>
                     <xdr:row>42</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6027,9 +6027,9 @@
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>1619250</xdr:colOff>
+                    <xdr:colOff>1623060</xdr:colOff>
                     <xdr:row>43</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6043,15 +6043,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>85725</xdr:colOff>
+                    <xdr:colOff>83820</xdr:colOff>
                     <xdr:row>47</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>819150</xdr:colOff>
+                    <xdr:colOff>822960</xdr:colOff>
                     <xdr:row>49</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6067,13 +6067,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>37</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:rowOff>160020</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>39</xdr:row>
-                    <xdr:rowOff>66675</xdr:rowOff>
+                    <xdr:rowOff>68580</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6089,13 +6089,13 @@
                     <xdr:col>1</xdr:col>
                     <xdr:colOff>152400</xdr:colOff>
                     <xdr:row>26</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:rowOff>144780</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>885825</xdr:colOff>
+                    <xdr:colOff>883920</xdr:colOff>
                     <xdr:row>28</xdr:row>
-                    <xdr:rowOff>47625</xdr:rowOff>
+                    <xdr:rowOff>45720</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -6109,15 +6109,15 @@
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>161925</xdr:colOff>
+                    <xdr:colOff>160020</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>895350</xdr:colOff>
+                    <xdr:colOff>899160</xdr:colOff>
                     <xdr:row>22</xdr:row>
-                    <xdr:rowOff>57150</xdr:rowOff>
+                    <xdr:rowOff>60960</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>